<commit_message>
Updates xml for package update
</commit_message>
<xml_diff>
--- a/data-raw/metadata/Location_attributes.xlsx
+++ b/data-raw/metadata/Location_attributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\EDI_data_repos_to_upload\fish-food-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09CCC6A-BEE2-47AC-8B8C-A0F21CA69AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3E2F5E-43FA-4A61-BFAF-799DDB705EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10065" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{EA408BAE-6FB1-4BF4-81C8-CFC6B96C724F}"/>
+    <workbookView xWindow="3540" yWindow="405" windowWidth="16350" windowHeight="7875" xr2:uid="{EA408BAE-6FB1-4BF4-81C8-CFC6B96C724F}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>Longitude at sample site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habitat Type </t>
+  </si>
+  <si>
+    <t>Habitat type at each site</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Identified purpose of each site</t>
   </si>
 </sst>
 </file>
@@ -461,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F0F272-FCAA-47ED-AB17-DC169B8F2718}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,15 +581,49 @@
         <v>18</v>
       </c>
     </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{BA3C5E33-98F7-47D7-93C4-1300CC932B38}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{BA3C5E33-98F7-47D7-93C4-1300CC932B38}">
       <formula1>"string,boolean,decimal,float,double,duration,dateTime,time,date,gYearMonth,gYear,gMonthDay,gDay,gMonth"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{5696B8DF-1E1E-4425-85B8-84459E8CCD16}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{5696B8DF-1E1E-4425-85B8-84459E8CCD16}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{45C39947-F29E-441D-8724-D5844F949A6B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{45C39947-F29E-441D-8724-D5844F949A6B}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>